<commit_message>
working on data reader
</commit_message>
<xml_diff>
--- a/references/Asymm_v_T0_121323.xlsx
+++ b/references/Asymm_v_T0_121323.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprou/repos/tau_mts/reference_code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprou/repos/tau_mts/references/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CC73E7-F8BB-7F4D-ADFB-B9F8FCB71CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01B4D88-45F4-9E47-9FB2-60F0FCBA94F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="1420" windowWidth="40400" windowHeight="26300" activeTab="1" xr2:uid="{CA397DA7-6DCE-ED43-814C-21F747C9D96D}"/>
+    <workbookView xWindow="2960" yWindow="2420" windowWidth="26900" windowHeight="19980" xr2:uid="{CA397DA7-6DCE-ED43-814C-21F747C9D96D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3348,9 +3348,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3388,7 +3388,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3494,7 +3494,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3636,7 +3636,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3646,14 +3646,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDF56B8-0042-E944-BD59-37CB7E331232}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:I13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4206,7 +4209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4983FAE1-0D64-ED45-9B1E-D12DFF7D5407}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -4601,26 +4604,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="fa762a6f-4bb3-4cb0-a720-f318dab4a9ea" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bb69b376-5d76-417c-8bd2-2d24bdfdf616">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F86782CE24CF84CBBBB6BA617A95B12" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58168f9cddf8c4c4be4d2556037c186e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb69b376-5d76-417c-8bd2-2d24bdfdf616" xmlns:ns3="fa762a6f-4bb3-4cb0-a720-f318dab4a9ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="12357374cbe2a5688140370039f7a66d" ns2:_="" ns3:_="">
     <xsd:import namespace="bb69b376-5d76-417c-8bd2-2d24bdfdf616"/>
@@ -4857,26 +4840,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BC90EE2-3B5A-477F-A37D-FFB1413450AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fa762a6f-4bb3-4cb0-a720-f318dab4a9ea"/>
-    <ds:schemaRef ds:uri="bb69b376-5d76-417c-8bd2-2d24bdfdf616"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C96BA76-7738-4927-B32A-0FF187003393}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="fa762a6f-4bb3-4cb0-a720-f318dab4a9ea" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bb69b376-5d76-417c-8bd2-2d24bdfdf616">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCCFA7D0-9CE0-4F50-99DF-547263724E90}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4893,4 +4877,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C96BA76-7738-4927-B32A-0FF187003393}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BC90EE2-3B5A-477F-A37D-FFB1413450AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fa762a6f-4bb3-4cb0-a720-f318dab4a9ea"/>
+    <ds:schemaRef ds:uri="bb69b376-5d76-417c-8bd2-2d24bdfdf616"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>